<commit_message>
updating our classifire version to version 2
Changing some structure
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59C555-87B0-4585-A021-1CAB47B314A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6591B149-01B5-4036-B099-BD9A4F85AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10776" yWindow="1824" windowWidth="11580" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>model_V0</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>A 1 P 0</t>
+  </si>
+  <si>
+    <t>model_V2</t>
+  </si>
+  <si>
+    <t>model_V3</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F7" sqref="A6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,6 +471,36 @@
         <v>0.159</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>449</v>
+      </c>
+      <c r="C4">
+        <v>578</v>
+      </c>
+      <c r="D4">
+        <v>540</v>
+      </c>
+      <c r="E4" s="1">
+        <v>433</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B4:E4)</f>
+        <v>2000</v>
+      </c>
+      <c r="G4" s="2">
+        <f>E4/F4</f>
+        <v>0.2165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating our model V3
Changing the hidden layers
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6591B149-01B5-4036-B099-BD9A4F85AF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4792D84-FED5-462D-B4E4-B4AEE3DF98FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10776" yWindow="1824" windowWidth="11580" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>model_V0</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>model_V3</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F7" sqref="A6:F7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,6 +423,9 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -499,6 +505,26 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
+      </c>
+      <c r="B5">
+        <v>225</v>
+      </c>
+      <c r="C5">
+        <v>774</v>
+      </c>
+      <c r="D5">
+        <v>764</v>
+      </c>
+      <c r="E5" s="1">
+        <v>237</v>
+      </c>
+      <c r="F5">
+        <f>SUM(B5:E5)</f>
+        <v>2000</v>
+      </c>
+      <c r="G5" s="2">
+        <f>E5/F5</f>
+        <v>0.11849999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating our model to version 4
adding more hidden layer to structure 7 dense hidden layer
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4792D84-FED5-462D-B4E4-B4AEE3DF98FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE754D9-D8A0-4011-8CAC-E7ECCB2D3DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>model_V0</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>model_V4</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,9 +411,10 @@
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -427,7 +431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -451,8 +455,16 @@
         <f>E2/F2</f>
         <v>0.25</v>
       </c>
+      <c r="I2">
+        <f>E2+D2</f>
+        <v>966</v>
+      </c>
+      <c r="J2" s="2">
+        <f>I2/F2</f>
+        <v>0.48299999999999998</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -476,8 +488,16 @@
         <f>E3/F3</f>
         <v>0.159</v>
       </c>
+      <c r="I3">
+        <f>E3+D3</f>
+        <v>1000</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J6" si="0">I3/F3</f>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -501,8 +521,16 @@
         <f>E4/F4</f>
         <v>0.2165</v>
       </c>
+      <c r="I4">
+        <f>E4+D4</f>
+        <v>973</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.48649999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -525,6 +553,47 @@
       <c r="G5" s="2">
         <f>E5/F5</f>
         <v>0.11849999999999999</v>
+      </c>
+      <c r="I5">
+        <f>E5+D5</f>
+        <v>1001</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.50049999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1011</v>
+      </c>
+      <c r="D6">
+        <v>989</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>SUM(B6:E6)</f>
+        <v>2000</v>
+      </c>
+      <c r="G6" s="2">
+        <f>E6/F6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>E6+D6</f>
+        <v>989</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the model to version 5
Checking if adding more hidden layer make our model improve or not
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F4F0DD-8F9C-4EB2-BD84-C287A9F8455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988D9275-38E4-47E8-968D-8E0EEB69057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>model_V0</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>model_V4.1</t>
+  </si>
+  <si>
+    <t>model_V5</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,6 +635,39 @@
         <v>0.4945</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1011</v>
+      </c>
+      <c r="D8">
+        <v>989</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>SUM(B8:E8)</f>
+        <v>2000</v>
+      </c>
+      <c r="G8" s="2">
+        <f>E8/F8</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>E8+D8</f>
+        <v>989</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8" si="2">I8/F8</f>
+        <v>0.4945</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the model to V6
Changing the hidden layer architecture to find the best possible option that i can find
Layer (type)                Output Shape              Param #
=================================================================
 dense (Dense)               (None, 128)               1792

 dropout (Dropout)           (None, 128)               0

 dense_1 (Dense)             (None, 64)                8256

 dense_2 (Dense)             (None, 64)                4160

 dense_3 (Dense)             (None, 64)                4160

 dense_4 (Dense)             (None, 64)                4160

 dense_5 (Dense)             (None, 1)                 65

==============================================================
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988D9275-38E4-47E8-968D-8E0EEB69057E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FBD32F-E728-4E2C-B178-3E9AA54B6AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>model_V0</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>model_V5</t>
+  </si>
+  <si>
+    <t>model_V6</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,6 +671,39 @@
         <v>0.4945</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1011</v>
+      </c>
+      <c r="D9">
+        <v>989</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>SUM(B9:E9)</f>
+        <v>2000</v>
+      </c>
+      <c r="G9" s="2">
+        <f>E9/F9</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>E9+D9</f>
+        <v>989</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" ref="J9" si="3">I9/F9</f>
+        <v>0.4945</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the model to V7
Reducing the hidden layers

Model Summary:
Model: "sequential"
_________________________________________________________________
 Layer (type)                Output Shape              Param #
=================================================================
 dense (Dense)               (None, 128)               1792

 dropout (Dropout)           (None, 128)               0

 dense_1 (Dense)             (None, 64)                8256

 dense_2 (Dense)             (None, 64)                4160

 dense_3 (Dense)             (None, 64)                4160

 dense_4 (Dense)             (None, 1)                 65

=================================================================
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FBD32F-E728-4E2C-B178-3E9AA54B6AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AD45A-AAD5-413E-BC08-F8FB31433F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>model_V0</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>model_V6</t>
+  </si>
+  <si>
+    <t>Lower hidden layers</t>
+  </si>
+  <si>
+    <t>model_V7</t>
+  </si>
+  <si>
+    <t>4 hidden layers</t>
+  </si>
+  <si>
+    <t>6 hidden layer</t>
+  </si>
+  <si>
+    <t>8 hidden layers</t>
   </si>
 </sst>
 </file>
@@ -407,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +438,7 @@
     <col min="10" max="10" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -440,7 +455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -473,7 +488,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -506,7 +521,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -539,7 +554,7 @@
         <v>0.48649999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -572,7 +587,7 @@
         <v>0.50049999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -604,8 +619,11 @@
         <f t="shared" si="0"/>
         <v>0.4945</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -637,8 +655,11 @@
         <f t="shared" ref="J7" si="1">I7/F7</f>
         <v>0.4945</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -670,8 +691,11 @@
         <f t="shared" ref="J8" si="2">I8/F8</f>
         <v>0.4945</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -702,6 +726,45 @@
       <c r="J9" s="2">
         <f t="shared" ref="J9" si="3">I9/F9</f>
         <v>0.4945</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>382</v>
+      </c>
+      <c r="C10">
+        <v>625</v>
+      </c>
+      <c r="D10">
+        <v>607</v>
+      </c>
+      <c r="E10" s="1">
+        <v>386</v>
+      </c>
+      <c r="F10">
+        <f>SUM(B10:E10)</f>
+        <v>2000</v>
+      </c>
+      <c r="G10" s="2">
+        <f>E10/F10</f>
+        <v>0.193</v>
+      </c>
+      <c r="I10">
+        <f>E10+D10</f>
+        <v>993</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" ref="J10" si="4">I10/F10</f>
+        <v>0.4965</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating our confusion Matrix
Adding some function to our excell
</commit_message>
<xml_diff>
--- a/Neural Network Classifier0/Matrix.xlsx
+++ b/Neural Network Classifier0/Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acking\Desktop\project\AI-Powered-River-Flood-Prediction-\Neural Network Classifier0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AD45A-AAD5-413E-BC08-F8FB31433F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36987DC-2967-4AE3-AA8C-B37929373586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>model_V0</t>
   </si>
@@ -42,18 +42,6 @@
     <t>model_V1</t>
   </si>
   <si>
-    <t xml:space="preserve">A 0 P 0 </t>
-  </si>
-  <si>
-    <t>A 1 P 1</t>
-  </si>
-  <si>
-    <t>A 0 P 1</t>
-  </si>
-  <si>
-    <t>A 1 P 0</t>
-  </si>
-  <si>
     <t>model_V2</t>
   </si>
   <si>
@@ -75,19 +63,25 @@
     <t>model_V6</t>
   </si>
   <si>
-    <t>Lower hidden layers</t>
-  </si>
-  <si>
     <t>model_V7</t>
   </si>
   <si>
-    <t>4 hidden layers</t>
-  </si>
-  <si>
-    <t>6 hidden layer</t>
-  </si>
-  <si>
-    <t>8 hidden layers</t>
+    <t xml:space="preserve">Test numbers </t>
+  </si>
+  <si>
+    <t>Actual 0 _Predicted 0</t>
+  </si>
+  <si>
+    <t>Actual 1_Predicted 1</t>
+  </si>
+  <si>
+    <t>Actual 0_Predicted 1</t>
+  </si>
+  <si>
+    <t>Actual 1_Predicted 0</t>
+  </si>
+  <si>
+    <t>Model Version</t>
   </si>
 </sst>
 </file>
@@ -110,18 +104,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,16 +125,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -157,6 +178,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{123270A3-EEE2-4620-A93C-EDDF36B4FC8B}" name="Table5" displayName="Table5" ref="A1:G10" totalsRowShown="0">
+  <autoFilter ref="A1:G10" xr:uid="{123270A3-EEE2-4620-A93C-EDDF36B4FC8B}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{74F1EA69-10BF-41AB-BA95-122A6A1A2A9D}" name="Model Version"/>
+    <tableColumn id="2" xr3:uid="{DFB3801A-00A8-4359-9642-6B26689CE181}" name="Actual 0 _Predicted 0"/>
+    <tableColumn id="3" xr3:uid="{30275CBD-28D0-40F0-BB1A-27811C276AE5}" name="Actual 1_Predicted 1"/>
+    <tableColumn id="4" xr3:uid="{C1D0F3AC-7B9F-4147-8872-700BEB3EEB76}" name="Actual 0_Predicted 1"/>
+    <tableColumn id="5" xr3:uid="{82C72620-E737-471E-9D41-E2BFFB6E55AE}" name="Actual 1_Predicted 0" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{92914AC3-E9BA-4EB9-904E-0972B7423B66}" name="Test numbers ">
+      <calculatedColumnFormula>SUM(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{33D1F99D-0677-4F11-B65F-3264C2D86396}" name="Error" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>E2/F2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,40 +463,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E10"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -468,27 +516,19 @@
       <c r="D2">
         <v>466</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>500</v>
       </c>
       <c r="F2">
         <f>SUM(B2:E2)</f>
         <v>2000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <f>E2/F2</f>
         <v>0.25</v>
       </c>
-      <c r="I2">
-        <f>E2+D2</f>
-        <v>966</v>
-      </c>
-      <c r="J2" s="2">
-        <f>I2/F2</f>
-        <v>0.48299999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -501,29 +541,21 @@
       <c r="D3">
         <v>682</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>318</v>
       </c>
       <c r="F3">
         <f>SUM(B3:E3)</f>
         <v>2000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f>E3/F3</f>
         <v>0.159</v>
       </c>
-      <c r="I3">
-        <f>E3+D3</f>
-        <v>1000</v>
-      </c>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J6" si="0">I3/F3</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>449</v>
@@ -534,29 +566,21 @@
       <c r="D4">
         <v>540</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>433</v>
       </c>
       <c r="F4">
         <f>SUM(B4:E4)</f>
         <v>2000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>E4/F4</f>
         <v>0.2165</v>
       </c>
-      <c r="I4">
-        <f>E4+D4</f>
-        <v>973</v>
-      </c>
-      <c r="J4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48649999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>225</v>
@@ -567,29 +591,21 @@
       <c r="D5">
         <v>764</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>237</v>
       </c>
       <c r="F5">
         <f>SUM(B5:E5)</f>
         <v>2000</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>E5/F5</f>
         <v>0.11849999999999999</v>
       </c>
-      <c r="I5">
-        <f>E5+D5</f>
-        <v>1001</v>
-      </c>
-      <c r="J5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.50049999999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -600,32 +616,21 @@
       <c r="D6">
         <v>989</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6">
         <f>SUM(B6:E6)</f>
         <v>2000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f>E6/F6</f>
         <v>0</v>
       </c>
-      <c r="I6">
-        <f>E6+D6</f>
-        <v>989</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.4945</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -636,32 +641,21 @@
       <c r="D7">
         <v>989</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7">
         <f>SUM(B7:E7)</f>
         <v>2000</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f>E7/F7</f>
         <v>0</v>
       </c>
-      <c r="I7">
-        <f>E7+D7</f>
-        <v>989</v>
-      </c>
-      <c r="J7" s="2">
-        <f t="shared" ref="J7" si="1">I7/F7</f>
-        <v>0.4945</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -672,32 +666,21 @@
       <c r="D8">
         <v>989</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
       <c r="F8">
         <f>SUM(B8:E8)</f>
         <v>2000</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f>E8/F8</f>
         <v>0</v>
       </c>
-      <c r="I8">
-        <f>E8+D8</f>
-        <v>989</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8" si="2">I8/F8</f>
-        <v>0.4945</v>
-      </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -708,32 +691,21 @@
       <c r="D9">
         <v>989</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9">
         <f>SUM(B9:E9)</f>
         <v>2000</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f>E9/F9</f>
         <v>0</v>
       </c>
-      <c r="I9">
-        <f>E9+D9</f>
-        <v>989</v>
-      </c>
-      <c r="J9" s="2">
-        <f t="shared" ref="J9" si="3">I9/F9</f>
-        <v>0.4945</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>382</v>
@@ -744,30 +716,22 @@
       <c r="D10">
         <v>607</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>386</v>
       </c>
       <c r="F10">
         <f>SUM(B10:E10)</f>
         <v>2000</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f>E10/F10</f>
         <v>0.193</v>
       </c>
-      <c r="I10">
-        <f>E10+D10</f>
-        <v>993</v>
-      </c>
-      <c r="J10" s="2">
-        <f t="shared" ref="J10" si="4">I10/F10</f>
-        <v>0.4965</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>